<commit_message>
partial update - additional objectives for Alvi
</commit_message>
<xml_diff>
--- a/BIRDSHOT-HEADATA-Alvi/Training-Avg2/results0/model_predictions1.xlsx
+++ b/BIRDSHOT-HEADATA-Alvi/Training-Avg2/results0/model_predictions1.xlsx
@@ -402,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -469,7 +469,7 @@
         <v>1.13</v>
       </c>
       <c r="J2">
-        <v>1.149133205413818</v>
+        <v>1.157105445861816</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -501,7 +501,7 @@
         <v>1.22</v>
       </c>
       <c r="J3">
-        <v>1.178200244903564</v>
+        <v>1.147045969963074</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -533,7 +533,7 @@
         <v>1.2</v>
       </c>
       <c r="J4">
-        <v>1.16866934299469</v>
+        <v>1.1449134349823</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -565,7 +565,7 @@
         <v>1.09</v>
       </c>
       <c r="J5">
-        <v>1.131289958953857</v>
+        <v>1.141607761383057</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -573,63 +573,63 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
       <c r="E6">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G6">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I6">
-        <v>1.14</v>
+        <v>1.13</v>
       </c>
       <c r="J6">
-        <v>1.149369239807129</v>
+        <v>1.138037204742432</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>4</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F7">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G7">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="H7">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>1.16</v>
+        <v>1.15</v>
       </c>
       <c r="J7">
-        <v>1.157520174980164</v>
+        <v>1.144461750984192</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -637,31 +637,31 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
       <c r="D8">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E8">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F8">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>1.2</v>
+        <v>1.14</v>
       </c>
       <c r="J8">
-        <v>1.165762186050415</v>
+        <v>1.129565715789795</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -672,28 +672,28 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
       <c r="E9">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="F9">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G9">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="H9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I9">
-        <v>1.17</v>
+        <v>1.16</v>
       </c>
       <c r="J9">
-        <v>1.159865379333496</v>
+        <v>1.141377806663513</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -701,63 +701,63 @@
         <v>4</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D10">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <v>8</v>
       </c>
       <c r="G10">
-        <v>48</v>
+        <v>56.00000000000001</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I10">
-        <v>1.17</v>
+        <v>1.09</v>
       </c>
       <c r="J10">
-        <v>1.154852747917175</v>
+        <v>1.133561730384827</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F11">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G11">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="H11">
         <v>4</v>
       </c>
       <c r="I11">
-        <v>1.13</v>
+        <v>1.2</v>
       </c>
       <c r="J11">
-        <v>1.14979088306427</v>
+        <v>1.146995663642883</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -765,7 +765,7 @@
         <v>4</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>8</v>
@@ -774,118 +774,118 @@
         <v>4</v>
       </c>
       <c r="E12">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F12">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G12">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I12">
-        <v>1.18</v>
+        <v>1.17</v>
       </c>
       <c r="J12">
-        <v>1.159217715263367</v>
+        <v>1.138037204742432</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F13">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G13">
         <v>48</v>
       </c>
       <c r="H13">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>1.15</v>
+        <v>1.17</v>
       </c>
       <c r="J13">
-        <v>1.143091440200806</v>
+        <v>1.131285071372986</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B14">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>4</v>
       </c>
       <c r="E14">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G14">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H14">
         <v>4</v>
       </c>
       <c r="I14">
-        <v>1.17</v>
+        <v>1.11</v>
       </c>
       <c r="J14">
-        <v>1.156838655471802</v>
+        <v>1.143470644950867</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B15">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D15">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E15">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G15">
         <v>44</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I15">
-        <v>1.09</v>
+        <v>1.13</v>
       </c>
       <c r="J15">
-        <v>1.15222442150116</v>
+        <v>1.143470644950867</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -896,28 +896,28 @@
         <v>12</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F16">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G16">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="H16">
         <v>8</v>
       </c>
       <c r="I16">
-        <v>1.17</v>
+        <v>1.07</v>
       </c>
       <c r="J16">
-        <v>1.163519859313965</v>
+        <v>1.132963418960571</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -925,63 +925,63 @@
         <v>4</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F17">
         <v>8</v>
       </c>
       <c r="G17">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H17">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>1.16</v>
+        <v>1.18</v>
       </c>
       <c r="J17">
-        <v>1.157101154327393</v>
+        <v>1.133069515228271</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B18">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C18">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>4</v>
       </c>
       <c r="F18">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="G18">
-        <v>39.99999999999999</v>
+        <v>48</v>
       </c>
       <c r="H18">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="I18">
-        <v>1.14</v>
+        <v>1.15</v>
       </c>
       <c r="J18">
-        <v>1.155028939247131</v>
+        <v>1.142873764038086</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -989,42 +989,42 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C19">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F19">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G19">
         <v>52</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I19">
-        <v>1.16</v>
+        <v>1.17</v>
       </c>
       <c r="J19">
-        <v>1.160130262374878</v>
+        <v>1.134259939193726</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B20">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C20">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D20">
         <v>4</v>
@@ -1033,19 +1033,19 @@
         <v>16</v>
       </c>
       <c r="F20">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G20">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I20">
-        <v>1.17</v>
+        <v>1.07</v>
       </c>
       <c r="J20">
-        <v>1.162884950637817</v>
+        <v>1.135977029800415</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1056,28 +1056,28 @@
         <v>12</v>
       </c>
       <c r="C21">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E21">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F21">
         <v>8</v>
       </c>
       <c r="G21">
-        <v>56.00000000000001</v>
+        <v>44</v>
       </c>
       <c r="H21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>1.12</v>
+        <v>1.09</v>
       </c>
       <c r="J21">
-        <v>1.147902607917786</v>
+        <v>1.132493495941162</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1085,31 +1085,31 @@
         <v>4</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E22">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F22">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G22">
-        <v>56.00000000000001</v>
+        <v>44</v>
       </c>
       <c r="H22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>1.14</v>
+        <v>1.13</v>
       </c>
       <c r="J22">
-        <v>1.152618050575256</v>
+        <v>1.132493495941162</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1117,7 +1117,7 @@
         <v>0</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C23">
         <v>8</v>
@@ -1132,21 +1132,21 @@
         <v>20</v>
       </c>
       <c r="G23">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H23">
         <v>4</v>
       </c>
       <c r="I23">
-        <v>1.17</v>
+        <v>1.09</v>
       </c>
       <c r="J23">
-        <v>1.160061597824097</v>
+        <v>1.145846128463745</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B24">
         <v>12</v>
@@ -1155,57 +1155,57 @@
         <v>4</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E24">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F24">
         <v>16</v>
       </c>
       <c r="G24">
-        <v>39.99999999999999</v>
+        <v>32</v>
       </c>
       <c r="H24">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I24">
         <v>1.17</v>
       </c>
       <c r="J24">
-        <v>1.151123285293579</v>
+        <v>1.148582100868225</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C25">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F25">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G25">
         <v>52</v>
       </c>
       <c r="H25">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="I25">
-        <v>1.14</v>
+        <v>1.16</v>
       </c>
       <c r="J25">
-        <v>1.152158498764038</v>
+        <v>1.140995979309082</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1213,63 +1213,63 @@
         <v>4</v>
       </c>
       <c r="B26">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C26">
         <v>4</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F26">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G26">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="H26">
         <v>12</v>
       </c>
       <c r="I26">
-        <v>1.21</v>
+        <v>1.07</v>
       </c>
       <c r="J26">
-        <v>1.168174386024475</v>
+        <v>1.130550265312195</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>12</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
         <v>24</v>
       </c>
-      <c r="C27">
-        <v>8</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>12</v>
-      </c>
-      <c r="F27">
-        <v>16</v>
-      </c>
       <c r="G27">
-        <v>32</v>
+        <v>39.99999999999999</v>
       </c>
       <c r="H27">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I27">
-        <v>1.15</v>
+        <v>1.14</v>
       </c>
       <c r="J27">
-        <v>1.157973289489746</v>
+        <v>1.147534132003784</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1277,95 +1277,95 @@
         <v>4</v>
       </c>
       <c r="B28">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="C28">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D28">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E28">
         <v>4</v>
       </c>
       <c r="F28">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G28">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="H28">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I28">
         <v>1.16</v>
       </c>
       <c r="J28">
-        <v>1.155263066291809</v>
+        <v>1.135774731636047</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B29">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E29">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F29">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G29">
         <v>36</v>
       </c>
       <c r="H29">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I29">
-        <v>1.18</v>
+        <v>1.17</v>
       </c>
       <c r="J29">
-        <v>1.165196180343628</v>
+        <v>1.144461750984192</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B30">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F30">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G30">
-        <v>28</v>
+        <v>56.00000000000001</v>
       </c>
       <c r="H30">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I30">
-        <v>1.17</v>
+        <v>1.12</v>
       </c>
       <c r="J30">
-        <v>1.159394502639771</v>
+        <v>1.133561730384827</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1373,31 +1373,479 @@
         <v>4</v>
       </c>
       <c r="B31">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E31">
         <v>16</v>
       </c>
       <c r="F31">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G31">
+        <v>56.00000000000001</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+      <c r="I31">
+        <v>1.14</v>
+      </c>
+      <c r="J31">
+        <v>1.133142948150635</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <v>16</v>
+      </c>
+      <c r="F32">
+        <v>20</v>
+      </c>
+      <c r="G32">
+        <v>44</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32">
+        <v>1.17</v>
+      </c>
+      <c r="J32">
+        <v>1.144545674324036</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>12</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>16</v>
+      </c>
+      <c r="G33">
+        <v>39.99999999999999</v>
+      </c>
+      <c r="H33">
+        <v>24</v>
+      </c>
+      <c r="I33">
+        <v>1.17</v>
+      </c>
+      <c r="J33">
+        <v>1.146426558494568</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="E34">
+        <v>16</v>
+      </c>
+      <c r="F34">
+        <v>12</v>
+      </c>
+      <c r="G34">
         <v>52</v>
       </c>
-      <c r="H31">
-        <v>8</v>
-      </c>
-      <c r="I31">
+      <c r="H34">
+        <v>8</v>
+      </c>
+      <c r="I34">
+        <v>1.1</v>
+      </c>
+      <c r="J34">
+        <v>1.139317631721497</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>16</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="E35">
+        <v>20</v>
+      </c>
+      <c r="F35">
+        <v>20</v>
+      </c>
+      <c r="G35">
+        <v>28</v>
+      </c>
+      <c r="H35">
+        <v>12</v>
+      </c>
+      <c r="I35">
         <v>1.13</v>
       </c>
-      <c r="J31">
-        <v>1.153608202934265</v>
+      <c r="J35">
+        <v>1.149639368057251</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <v>16</v>
+      </c>
+      <c r="C36">
+        <v>8</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>12</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>48</v>
+      </c>
+      <c r="H36">
+        <v>12</v>
+      </c>
+      <c r="I36">
+        <v>1.08</v>
+      </c>
+      <c r="J36">
+        <v>1.133115649223328</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>8</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>16</v>
+      </c>
+      <c r="F37">
+        <v>12</v>
+      </c>
+      <c r="G37">
+        <v>52</v>
+      </c>
+      <c r="H37">
+        <v>8</v>
+      </c>
+      <c r="I37">
+        <v>1.14</v>
+      </c>
+      <c r="J37">
+        <v>1.139317631721497</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="E38">
+        <v>12</v>
+      </c>
+      <c r="F38">
+        <v>16</v>
+      </c>
+      <c r="G38">
+        <v>36</v>
+      </c>
+      <c r="H38">
+        <v>12</v>
+      </c>
+      <c r="I38">
+        <v>1.21</v>
+      </c>
+      <c r="J38">
+        <v>1.150059700012207</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>24</v>
+      </c>
+      <c r="C39">
+        <v>8</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>12</v>
+      </c>
+      <c r="F39">
+        <v>16</v>
+      </c>
+      <c r="G39">
+        <v>32</v>
+      </c>
+      <c r="H39">
+        <v>8</v>
+      </c>
+      <c r="I39">
+        <v>1.15</v>
+      </c>
+      <c r="J39">
+        <v>1.153864145278931</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>32</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>20</v>
+      </c>
+      <c r="G40">
+        <v>24</v>
+      </c>
+      <c r="H40">
+        <v>4</v>
+      </c>
+      <c r="I40">
+        <v>1.16</v>
+      </c>
+      <c r="J40">
+        <v>1.150312781333923</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>24</v>
+      </c>
+      <c r="C41">
+        <v>8</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>12</v>
+      </c>
+      <c r="F41">
+        <v>16</v>
+      </c>
+      <c r="G41">
+        <v>32</v>
+      </c>
+      <c r="H41">
+        <v>8</v>
+      </c>
+      <c r="I41">
+        <v>1.25</v>
+      </c>
+      <c r="J41">
+        <v>1.153864145278931</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>40</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>12</v>
+      </c>
+      <c r="F42">
+        <v>4</v>
+      </c>
+      <c r="G42">
+        <v>36</v>
+      </c>
+      <c r="H42">
+        <v>4</v>
+      </c>
+      <c r="I42">
+        <v>1.18</v>
+      </c>
+      <c r="J42">
+        <v>1.157070159912109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>16</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <v>20</v>
+      </c>
+      <c r="F43">
+        <v>20</v>
+      </c>
+      <c r="G43">
+        <v>28</v>
+      </c>
+      <c r="H43">
+        <v>12</v>
+      </c>
+      <c r="I43">
+        <v>1.17</v>
+      </c>
+      <c r="J43">
+        <v>1.149639368057251</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>20</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>4</v>
+      </c>
+      <c r="E44">
+        <v>16</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>52</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>1.13</v>
+      </c>
+      <c r="J44">
+        <v>1.129565715789795</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45">
+        <v>12</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>16</v>
+      </c>
+      <c r="F45">
+        <v>8</v>
+      </c>
+      <c r="G45">
+        <v>52</v>
+      </c>
+      <c r="H45">
+        <v>8</v>
+      </c>
+      <c r="I45">
+        <v>1.13</v>
+      </c>
+      <c r="J45">
+        <v>1.132963418960571</v>
       </c>
     </row>
   </sheetData>
@@ -1407,7 +1855,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1474,7 +1922,7 @@
         <v>1.13</v>
       </c>
       <c r="J2">
-        <v>1.167481184005737</v>
+        <v>1.148463845252991</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1506,7 +1954,7 @@
         <v>1.15</v>
       </c>
       <c r="J3">
-        <v>1.148685097694397</v>
+        <v>1.133115649223328</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1514,31 +1962,31 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>4</v>
       </c>
       <c r="E4">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F4">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G4">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H4">
         <v>4</v>
       </c>
       <c r="I4">
-        <v>1.12</v>
+        <v>1.06</v>
       </c>
       <c r="J4">
-        <v>1.156157612800598</v>
+        <v>1.134259939193726</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1546,31 +1994,31 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F5">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G5">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I5">
-        <v>1.16</v>
+        <v>1.12</v>
       </c>
       <c r="J5">
-        <v>1.1678067445755</v>
+        <v>1.135977029800415</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1578,31 +2026,31 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G6">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="H6">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>1.14</v>
+        <v>1.16</v>
       </c>
       <c r="J6">
-        <v>1.15604293346405</v>
+        <v>1.151347041130066</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1619,22 +2067,22 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G7">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="H7">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I7">
-        <v>1.17</v>
+        <v>1.14</v>
       </c>
       <c r="J7">
-        <v>1.153967976570129</v>
+        <v>1.138009905815125</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1642,7 +2090,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -1651,22 +2099,22 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G8">
-        <v>39.99999999999999</v>
+        <v>52</v>
       </c>
       <c r="H8">
         <v>12</v>
       </c>
       <c r="I8">
-        <v>1.21</v>
+        <v>1.17</v>
       </c>
       <c r="J8">
-        <v>1.154049038887024</v>
+        <v>1.130550265312195</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1674,31 +2122,95 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G9">
+        <v>39.99999999999999</v>
+      </c>
+      <c r="H9">
+        <v>12</v>
+      </c>
+      <c r="I9">
+        <v>1.21</v>
+      </c>
+      <c r="J9">
+        <v>1.126288414001465</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10">
         <v>52</v>
       </c>
-      <c r="H9">
+      <c r="H10">
         <v>24</v>
       </c>
-      <c r="I9">
+      <c r="I10">
         <v>1.13</v>
       </c>
-      <c r="J9">
-        <v>1.157646536827087</v>
+      <c r="J10">
+        <v>1.141278505325317</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11">
+        <v>48</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1.14</v>
+      </c>
+      <c r="J11">
+        <v>1.133069396018982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>